<commit_message>
Just the presentation title left to go
Presentation.pptx got too big so it was added to the gitignore
</commit_message>
<xml_diff>
--- a/Data/IndividualCounties/4019.xlsx
+++ b/Data/IndividualCounties/4019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusli\Documents\GitHub\COVID-TimeSeries-GIS\Data\IndividualCounties\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guslipkin/Documents/COVID-TimeSeries-GIS/Data/IndividualCounties/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290B895B-2BA0-4DE2-A300-7B090711CB39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67A27083-383B-1444-98F3-EB22F73A76EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51200" yWindow="-6420" windowWidth="21600" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -543,11 +543,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -597,7 +599,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -647,7 +649,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -697,7 +699,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -747,7 +749,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -797,7 +799,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -847,7 +849,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -897,7 +899,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -947,7 +949,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -997,7 +999,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1047,7 +1049,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1097,7 +1099,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1147,7 +1149,7 @@
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1207,36 +1209,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D679EDBB-1260-4A48-9CD4-5332E2F6F8FB}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -1244,7 +1246,7 @@
         <v>0.51759719758797151</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -1252,7 +1254,7 @@
         <v>0.26790685895092164</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -1260,7 +1262,7 @@
         <v>-6.6280689424827455E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1268,7 +1270,7 @@
         <v>8331.3775842149553</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1276,12 +1278,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="3" t="s">
         <v>28</v>
@@ -1299,7 +1301,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -1319,7 +1321,7 @@
         <v>0.45068383655721833</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1335,7 +1337,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
@@ -1349,8 +1351,8 @@
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
     </row>
-    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
       <c r="B16" s="3" t="s">
         <v>33</v>
@@ -1377,7 +1379,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>27</v>
       </c>
@@ -1406,7 +1408,7 @@
         <v>339434.28624440928</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>40</v>
       </c>
@@ -1435,7 +1437,7 @@
         <v>433.06326188908474</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1464,7 +1466,7 @@
         <v>93984.028485225601</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>42</v>
       </c>
@@ -1493,13 +1495,13 @@
         <v>4998880.6471354589</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>44</v>
       </c>
@@ -1510,7 +1512,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>1</v>
       </c>
@@ -1521,7 +1523,7 @@
         <v>-6279.2108043148946</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>2</v>
       </c>
@@ -1532,7 +1534,7 @@
         <v>-8780.4612129908273</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>3</v>
       </c>
@@ -1543,7 +1545,7 @@
         <v>4709.0039429321423</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>4</v>
       </c>
@@ -1554,7 +1556,7 @@
         <v>-3616.0721472626064</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>5</v>
       </c>
@@ -1565,7 +1567,7 @@
         <v>-4416.5541785980995</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>6</v>
       </c>
@@ -1576,7 +1578,7 @@
         <v>294.98718763875331</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>7</v>
       </c>
@@ -1587,7 +1589,7 @@
         <v>3530.8496763595003</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>8</v>
       </c>
@@ -1598,7 +1600,7 @@
         <v>3205.7002176126202</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>9</v>
       </c>
@@ -1609,7 +1611,7 @@
         <v>-2959.3986520816279</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>10</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>-6946.1147159450429</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>11</v>
       </c>
@@ -1631,7 +1633,7 @@
         <v>4374.0200021521732</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>12</v>
       </c>

</xml_diff>